<commit_message>
add: workout page i18n
</commit_message>
<xml_diff>
--- a/LanguagePack.xlsx
+++ b/LanguagePack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choeinhwan/Desktop/Project/fitness-recoder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1596D9B9-FFEA-EB4B-ADDA-BAEB4FA236E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2566B1AE-DC1A-0140-A41F-2E7A3DCE614B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="93">
   <si>
     <t>namespace</t>
   </si>
@@ -285,6 +285,62 @@
   </si>
   <si>
     <t>홈</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>error</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>wrong.schedule</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Don't have schedule. Please, check again</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>잘못된 접근입니다. 스케줄을 확인해주세요.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>workout</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>actionBtn.start</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>actionBtn.pause</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>actionBtn.finish</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pause</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Finish</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>시작하기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>일시정지</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>종료</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -689,16 +745,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="2" width="38.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -874,76 +930,83 @@
     </row>
     <row r="15" spans="1:4" ht="16.5" customHeight="1"/>
     <row r="16" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
-      </c>
-    </row>
+      <c r="A16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" customHeight="1"/>
     <row r="18" spans="1:4" ht="16.5" customHeight="1"/>
     <row r="19" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A19" s="3" t="s">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="21" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>31</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>32</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A21" s="2"/>
     </row>
     <row r="22" spans="1:4" ht="16.5" customHeight="1">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.5" customHeight="1">
       <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A24" s="3"/>
+      <c r="A24" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A25" s="3"/>
+      <c r="A25" s="2"/>
     </row>
     <row r="26" spans="1:4" ht="16.5" customHeight="1">
       <c r="A26" s="3" t="s">
@@ -1075,6 +1138,48 @@
       </c>
       <c r="D37" t="s">
         <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" t="s">
+        <v>89</v>
+      </c>
+      <c r="D41" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add: delete exercise preset & start with Exercise Preset
</commit_message>
<xml_diff>
--- a/LanguagePack.xlsx
+++ b/LanguagePack.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choeinhwan/Desktop/Project/fitness-recoder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31562B4F-434A-C045-9B22-DB88F4A305E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79216A5A-58F6-E24F-98D8-723344CE24EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="116">
   <si>
     <t>namespace</t>
   </si>
@@ -394,6 +394,46 @@
   </si>
   <si>
     <t>프리셋으로 저장</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>menu.startWorkoutWithPreset</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start Workout</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>운동 시작</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>addExercise</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add Exercise</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>운동 추가</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>savePreset</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>menu.deletePreset</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete Preset</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>프리셋 삭제</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -449,11 +489,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -798,10 +837,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -995,312 +1034,367 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="16" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" t="s">
+        <v>111</v>
+      </c>
+    </row>
     <row r="17" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="19" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="20" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="21" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="22" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="23" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="24" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="25" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="26" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="27" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A27" t="s">
         <v>78</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B27" t="s">
         <v>79</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C27" t="s">
         <v>80</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D27" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16.5" customHeight="1"/>
-    <row r="19" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A19" t="s">
+    <row r="28" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="29" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A29" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C29" t="s">
         <v>28</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="16.5" customHeight="1"/>
-    <row r="21" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A21" s="3" t="s">
+    <row r="30" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="31" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B31" t="s">
         <v>31</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C31" t="s">
         <v>32</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A22" s="3" t="s">
+    <row r="32" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B32" t="s">
         <v>34</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C32" t="s">
         <v>35</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A24" s="3" t="s">
+    <row r="33" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="34" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B34" t="s">
         <v>38</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C34" t="s">
         <v>39</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A25" s="2"/>
-    </row>
-    <row r="26" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A26" s="3" t="s">
+    <row r="35" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="36" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A36" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B36" t="s">
         <v>41</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C36" t="s">
         <v>86</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A27" s="2"/>
-    </row>
-    <row r="28" spans="1:4" ht="16.5" customHeight="1">
-      <c r="A28" s="3" t="s">
+    <row r="37" spans="1:4" ht="16.5" customHeight="1"/>
+    <row r="38" spans="1:4" ht="16.5" customHeight="1">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B38" t="s">
         <v>43</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C38" t="s">
         <v>44</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D38" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="3" t="s">
+    <row r="39" spans="1:4">
+      <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B39" t="s">
         <v>46</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C39" t="s">
         <v>47</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="2"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
         <v>49</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B41" t="s">
         <v>65</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C41" t="s">
         <v>66</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D41" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
         <v>49</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B42" t="s">
         <v>53</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C42" t="s">
         <v>54</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D42" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>49</v>
-      </c>
-      <c r="B33" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>49</v>
-      </c>
-      <c r="B35" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="C43" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="D44" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D45" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" t="s">
-        <v>98</v>
-      </c>
-      <c r="D46" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="D47" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" t="s">
+        <v>92</v>
+      </c>
+      <c r="C48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" t="s">
+        <v>107</v>
+      </c>
+      <c r="D49" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
         <v>82</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B53" t="s">
+        <v>83</v>
+      </c>
+      <c r="C53" t="s">
+        <v>86</v>
+      </c>
+      <c r="D53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" t="s">
+        <v>87</v>
+      </c>
+      <c r="D54" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" t="s">
+        <v>82</v>
+      </c>
+      <c r="B55" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" t="s">
+        <v>88</v>
+      </c>
+      <c r="D55" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B56" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" t="s">
+        <v>98</v>
+      </c>
+      <c r="D56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>82</v>
+      </c>
+      <c r="B57" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" t="s">
+        <v>101</v>
+      </c>
+      <c r="D57" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" t="s">
         <v>103</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C58" t="s">
         <v>104</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D58" t="s">
         <v>105</v>
       </c>
     </row>

</xml_diff>